<commit_message>
1st documented defect fixes.
</commit_message>
<xml_diff>
--- a/documentation/defects.xlsx
+++ b/documentation/defects.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16ecbb52d5e766a3/Documents/TechStuff/Projects/Enlarger_Timer/FADU_Timer/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bob\OneDrive\Documents\TechStuff\Projects\Enlarger_Timer\FADU_Timer\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{3CBD49A9-EBAC-4436-B860-85F4D7170538}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{6FFCB9DF-B65B-40F3-9CFC-8794F08D8140}"/>
+  <xr:revisionPtr revIDLastSave="173" documentId="8_{3CBD49A9-EBAC-4436-B860-85F4D7170538}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{30620E5D-C959-45BD-A666-C2ADE622039B}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2820" windowWidth="24705" windowHeight="12015" xr2:uid="{736E6442-F76E-41A5-9606-E17F3A3051F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{736E6442-F76E-41A5-9606-E17F3A3051F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
-  <si>
-    <t>BUGS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Status</t>
   </si>
@@ -63,45 +60,18 @@
     <t>After 1st count, the count is &lt;&lt; 0.1s per tick.</t>
   </si>
   <si>
-    <t>Fix Description</t>
-  </si>
-  <si>
-    <t>Defect #</t>
-  </si>
-  <si>
     <t>STRIPS</t>
   </si>
   <si>
     <t>Any</t>
   </si>
   <si>
-    <t>Need to reset the timer to where it was when START was hit.</t>
-  </si>
-  <si>
-    <t>Hitting STOP in mid sequence leaves the timer in an undefined state.</t>
-  </si>
-  <si>
-    <t>Can move to another tab when strips timing is in progress</t>
-  </si>
-  <si>
-    <t>Need to reset the timer if move away from STRIPS tab mid-strip.</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
     <t>NS</t>
   </si>
   <si>
-    <t>IP</t>
-  </si>
-  <si>
-    <t>1st beep too low freq and too long - possibly too quiet</t>
-  </si>
-  <si>
-    <t>Should be higher freq (but lower than end-beep) and shorter.</t>
-  </si>
-  <si>
     <t>1.3.1</t>
   </si>
   <si>
@@ -111,43 +81,70 @@
     <t>FIX</t>
   </si>
   <si>
-    <t>Do not load this value on startup.  Forced user to set the strip base-time via the display and the SET button.</t>
-  </si>
-  <si>
     <t>Timer counting</t>
   </si>
   <si>
-    <t>When moving to Strips Mode, timer switches to STRIPS mode counting.</t>
-  </si>
-  <si>
-    <t>Count should stop and reset to STRIPS mode initialisation.</t>
-  </si>
-  <si>
-    <t>STRIPS / MAIN</t>
-  </si>
-  <si>
-    <t>Timer Counting</t>
-  </si>
-  <si>
-    <t>Moving from the STRIPS tab should reinitialise strips mode.</t>
-  </si>
-  <si>
-    <t>When moving to the MAIN timer tab from the STRIPS tab, any count in progress continues in main timer mode and stops at the end of the count, BUT strips mode settings remain in mid-process state.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Procedure "StartMainTimer" did not set START_MS if called by the clkCountIn.Timer block with count-in &gt; 0 (i.e. when we want a delay between strips). </t>
   </si>
   <si>
     <t>Strip mode = CONT; Settings-&gt;Delay &gt; 0 (i.e. Continuous mode with a delay between strips)</t>
   </si>
   <si>
-    <t>Strip mode = CONT; SETTINGS tab - Delay = 0 (i.e. Continuous mode with no delay between strips)</t>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>Ticks and beeps inconsitent in volume and frequency and length</t>
+  </si>
+  <si>
+    <t>Improve the quality of the sounds.</t>
+  </si>
+  <si>
+    <t>Release Note</t>
+  </si>
+  <si>
+    <t>Hitting STOP in mid Strips sequence leaves the timer in an undefined state.</t>
+  </si>
+  <si>
+    <t>Fix Requirements</t>
+  </si>
+  <si>
+    <t>When moving to Strips or Main timing mode tabs, the timer switches to the new mode. Timing is disrupted and confusing to the user.</t>
+  </si>
+  <si>
+    <t>Timer should always count in 100ms incements.</t>
+  </si>
+  <si>
+    <t>Do not load this value on startup.  Force user to set the strip base-time via the display and the SET button.</t>
+  </si>
+  <si>
+    <t>Value no longer loaded on startup.</t>
+  </si>
+  <si>
+    <t>Timer should not switch mode when changing tab.</t>
+  </si>
+  <si>
+    <t>New globals STRIPS_MODE _ENABLED and MAIN_MODE_ENABLED used to set the mode (previously relied on visibility of the Strips mode screen to detect which mode of timing to use).</t>
+  </si>
+  <si>
+    <t>DEFECTS AND ENHANCEMENTS</t>
+  </si>
+  <si>
+    <t>Issue Number</t>
+  </si>
+  <si>
+    <t>?  Do we need this.  Only an issue if not using hardware switching and user is unlikely to hit STOP by accident in CONT mode with no delay.  Also, if hit in CONT mode with no hardware switching user is stuffed anyway…</t>
+  </si>
+  <si>
+    <t>Lowered end-beep and incresed stripp-end warning beep frequencies. Tick shorter and colume incresed to fit other sounds better.  Trimmed silence.</t>
+  </si>
+  <si>
+    <t>Hitting [RST] in STRIPS mode should reload the strip base time value to allow a new strip-mode timing with the previous base time value.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -157,7 +154,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,13 +163,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8080"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -203,17 +194,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="21">
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -224,6 +215,9 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -247,10 +241,113 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="medium">
+          <color theme="1"/>
+        </left>
+        <right style="medium">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="TableStyleLight8 2" pivot="0" count="9" xr9:uid="{21596791-6411-4C89-98C7-8601619E2F76}">
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumn" dxfId="17"/>
+      <tableStyleElement type="lastColumn" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
+      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="12"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFF4040"/>
       <color rgb="FFFF8080"/>
     </mruColors>
   </colors>
@@ -266,20 +363,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6B85C10-F592-481D-A956-F7AFAE7B059C}" name="Table1" displayName="Table1" ref="A3:I16" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A3:I16" xr:uid="{5BF12587-82C4-494F-B99C-6BF1DD97078A}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{AB222748-23DB-4AE2-900B-3E79A9889B5F}" name="Defect #" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{05AE2F3A-1B3A-4EB5-8D69-4CC3F7B32BBA}" name="Priority" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{E4048DC5-3B10-4327-9134-3741C6B64273}" name="Status" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{C04235DD-C513-4CDD-BAF4-49DC0FC9B265}" name="Version Found" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{C2CEB40F-BA34-4F94-AF4B-CA7C16EA973B}" name="Version Fixed" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{9981D987-481D-43A0-A385-78D48791078B}" name="Screen" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{F8FBDE84-E169-4545-92CE-FD106BF001B3}" name="Settings" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{E5646472-8054-4F89-9283-2094DE6791CC}" name="Issue" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{72327442-8288-4FEA-851C-1C93F8CBDB3B}" name="Fix Description" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F6B85C10-F592-481D-A956-F7AFAE7B059C}" name="Table1" displayName="Table1" ref="A3:J13" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A3:J13" xr:uid="{5BF12587-82C4-494F-B99C-6BF1DD97078A}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{AB222748-23DB-4AE2-900B-3E79A9889B5F}" name="Issue Number" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{05AE2F3A-1B3A-4EB5-8D69-4CC3F7B32BBA}" name="Priority" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{E4048DC5-3B10-4327-9134-3741C6B64273}" name="Status" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{C04235DD-C513-4CDD-BAF4-49DC0FC9B265}" name="Version Found" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{C2CEB40F-BA34-4F94-AF4B-CA7C16EA973B}" name="Version Fixed" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9981D987-481D-43A0-A385-78D48791078B}" name="Screen" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{F8FBDE84-E169-4545-92CE-FD106BF001B3}" name="Settings" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{E5646472-8054-4F89-9283-2094DE6791CC}" name="Issue" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{72327442-8288-4FEA-851C-1C93F8CBDB3B}" name="Fix Requirements" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{7A56E528-2513-4793-B53C-514229CF7D1B}" name="Release Note" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight8 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -580,60 +678,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871DEB98-E520-4C60-BE88-D7878B15EB24}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41.5703125" customWidth="1"/>
     <col min="8" max="8" width="53" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="60.140625" customWidth="1"/>
+    <col min="9" max="9" width="51.7109375" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -641,193 +743,195 @@
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <f>A4+1</f>
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <f>A5+1</f>
+        <v>3</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="D6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>3</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="I6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <f t="shared" ref="A7:A13" si="0">A6+1</f>
+        <v>4</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1.33</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="G8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="I8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="J8" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -836,9 +940,13 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -847,9 +955,13 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -858,44 +970,13 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="J13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>